<commit_message>
final update to initial scraper
</commit_message>
<xml_diff>
--- a/ACT-IAC_Events-02.23.23.xlsx
+++ b/ACT-IAC_Events-02.23.23.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jorcas/Development/python_scraper_parser_projects/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D852C9B8-71CF-1A43-B245-23D49FF46049}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="38440" yWindow="500" windowWidth="30200" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -172,13 +178,13 @@
     <t>Join the ACT-IAC IT Management and Modernization COI March 2023 meeting. Additional event information will be available soon.</t>
   </si>
   <si>
-    <t xml:space="preserve">The Voyager Class of 2023 invites all Fellows to Voyagers Got Talent showcasing the incredible talents of this year's Voyager Class. </t>
+    <t>The Voyager Class of 2023 invites all Fellows to Voyagers Got Talent showcasing the incredible talents of this year's Voyager Class. </t>
   </si>
   <si>
     <t>Join the ACT-IAC Cyber COI member meeting to hear from an invited government speakers Heather Kowalski, CIO, Interpol, Department of Justice, and Dr. Tiina KO Rodrigue, CISO, CFPB</t>
   </si>
   <si>
-    <t xml:space="preserve">This program is being planned by the Department of Education Federal Insights Exchange (FIE) planning team. </t>
+    <t>This program is being planned by the Department of Education Federal Insights Exchange (FIE) planning team. </t>
   </si>
   <si>
     <t>Join the ACT-IAC Evolving the Workforce COI March 2023 member meeting. More information about topic " The ABCs of Recruiting Gen Z" and speaker/s will be available soon.</t>
@@ -247,8 +253,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,9 +294,14 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -298,6 +309,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -344,7 +363,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -376,9 +395,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -410,6 +447,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -585,371 +640,377 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="28.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="4" width="28.33203125" style="1"/>
+    <col min="5" max="5" width="57" style="1" customWidth="1"/>
+    <col min="6" max="6" width="56.6640625" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="28.33203125" style="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
-      <c r="A6" t="s">
+    <row r="6" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
-      <c r="A7" t="s">
+    <row r="7" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
-      <c r="A8" t="s">
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
-      <c r="A9" t="s">
+    <row r="9" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
-      <c r="A10" t="s">
+    <row r="10" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="E10" t="s">
+      <c r="E10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
-      <c r="A11" t="s">
+    <row r="11" spans="1:6" ht="64" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E11" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
-      <c r="A12" t="s">
+    <row r="12" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
-      <c r="A13" t="s">
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
-      <c r="A14" t="s">
+    <row r="14" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E14" t="s">
+      <c r="E14" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
-      <c r="A15" t="s">
+    <row r="15" spans="1:6" ht="48" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E15" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
-      <c r="A16" t="s">
+    <row r="16" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
-      <c r="A17" t="s">
+    <row r="17" spans="1:6" ht="32" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E17" t="s">
+      <c r="E17" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
+    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="2" t="s">
         <v>75</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
-    <hyperlink ref="F5" r:id="rId4"/>
-    <hyperlink ref="F6" r:id="rId5"/>
-    <hyperlink ref="F7" r:id="rId6"/>
-    <hyperlink ref="F8" r:id="rId7"/>
-    <hyperlink ref="F9" r:id="rId8"/>
-    <hyperlink ref="F10" r:id="rId9"/>
-    <hyperlink ref="F11" r:id="rId10"/>
-    <hyperlink ref="F12" r:id="rId11"/>
-    <hyperlink ref="F13" r:id="rId12"/>
-    <hyperlink ref="F14" r:id="rId13"/>
-    <hyperlink ref="F15" r:id="rId14"/>
-    <hyperlink ref="F16" r:id="rId15"/>
-    <hyperlink ref="F17" r:id="rId16"/>
-    <hyperlink ref="F18" r:id="rId17"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="F3" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="F4" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="F5" r:id="rId4" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="F6" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="F11" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="F12" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="F13" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="F14" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="F15" r:id="rId14" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="F16" r:id="rId15" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="F17" r:id="rId16" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="F18" r:id="rId17" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>